<commit_message>
geracao das notas finais html
</commit_message>
<xml_diff>
--- a/Projeto_4bim/NOTASFINAISALUNOS.xlsx
+++ b/Projeto_4bim/NOTASFINAISALUNOS.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -755,6 +755,166 @@
         <v>4</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>50230552</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>thiago</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>7</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>54023320</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>val</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" t="n">
+        <v>42</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>12</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>aprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>50230552</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>thiago</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" t="n">
+        <v>5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>423</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>thiago</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>val</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5</v>
+      </c>
+      <c r="G17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>reprovado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>